<commit_message>
Added analysis of filtered reviews, those by reviewers with > 5 reviews.
</commit_message>
<xml_diff>
--- a/level-2/bias_analysis.xlsx
+++ b/level-2/bias_analysis.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6bacb2ee70178176/Personal/UCSD_Data_Science_Bootcamp/Homework/2020-05-04_HW22_BigData/big-data-challenge/level-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{71BE7603-BA9E-FF47-B49B-8042B597E0F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DD006C28-073C-444C-8DD5-B7CA4D3439B5}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="8_{71BE7603-BA9E-FF47-B49B-8042B597E0F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{3D3DADE1-C793-B547-9CE5-67E452D2485E}"/>
   <bookViews>
-    <workbookView xWindow="8960" yWindow="3240" windowWidth="27880" windowHeight="18720" xr2:uid="{8766E0C5-1C09-C443-BEE9-386DCCD50C69}"/>
+    <workbookView xWindow="15220" yWindow="1020" windowWidth="21540" windowHeight="20980" activeTab="1" xr2:uid="{8766E0C5-1C09-C443-BEE9-386DCCD50C69}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="All Reviews" sheetId="1" r:id="rId1"/>
+    <sheet name="Filtered Reviews" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="26">
   <si>
     <t>rating_sd</t>
   </si>
@@ -133,18 +134,48 @@
       <t>The T-stat/p-value is significant, therefore we reject the null and conclude that there is a meaningful difference in the average ratings of Vine reviewers and non-vine reviewers</t>
     </r>
   </si>
+  <si>
+    <t>See the next tab for filtered reviews.</t>
+  </si>
+  <si>
+    <t>Filtered reviews: Only those where the reviewer posted 5 or more reviews are included. Video_games only!</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Conclusion: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The null hypothesis is NOT rejectec when reviews are filtered to only those by customers who have posted 5 or more reviews. In fact, Vine reviewers have notably lower review scores! Note that due to the structure of our dataset, we're only looking at reviews of video games in this case.</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="174" formatCode="0.00000"/>
-    <numFmt numFmtId="177" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.00000"/>
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="170" formatCode="0.000%"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -179,13 +210,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -202,19 +247,22 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -327,6 +375,99 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>426355</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>119453</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>442684</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>453570</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDFB63AC-22A0-4146-8254-0E6BAB883446}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5011055" y="1237053"/>
+          <a:ext cx="5794829" cy="3991717"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>562429</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>163285</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>524329</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>52614</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{920179C0-CDC3-8C4B-8679-2F205EBA4E71}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5147129" y="5814785"/>
+          <a:ext cx="3263900" cy="1514929"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{292DA351-94C7-6E4B-B49E-6540012004F3}" name="Table1" displayName="Table1" ref="A7:D9" totalsRowShown="0">
   <autoFilter ref="A7:D9" xr:uid="{91C61CCF-DF69-1649-940D-A4CDE5C12928}"/>
@@ -335,6 +476,19 @@
     <tableColumn id="2" xr3:uid="{B82B8A05-AC99-BB4D-803C-9C93A63BCB6C}" name="count"/>
     <tableColumn id="3" xr3:uid="{E4415B70-5680-9941-AB6E-308706610B1F}" name="rating_mean"/>
     <tableColumn id="4" xr3:uid="{CCAC6381-85FD-EE44-89FB-01496C14704C}" name="rating_sd"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{A239AA40-DD5D-1E46-AC75-28B7B2CC656C}" name="Table13" displayName="Table13" ref="A7:D9" totalsRowShown="0">
+  <autoFilter ref="A7:D9" xr:uid="{91C61CCF-DF69-1649-940D-A4CDE5C12928}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{99FEF5D4-251A-C848-ADDB-0B5417F08C5A}" name="vine"/>
+    <tableColumn id="2" xr3:uid="{DB36BAAC-8BE9-9C4F-93D8-0477EF0BC8C0}" name="count"/>
+    <tableColumn id="3" xr3:uid="{9DADBE8D-7847-3249-9190-9C7A05DF896D}" name="rating_mean"/>
+    <tableColumn id="4" xr3:uid="{2F97F45F-0924-804E-9163-87261395521B}" name="rating_sd"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -637,10 +791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A151E979-AE21-7048-9135-6CF3F729192B}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -651,7 +805,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -814,12 +968,226 @@
       </c>
     </row>
     <row r="24" spans="1:4" ht="69" customHeight="1">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="8"/>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A24:D24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C3EBED-4E1F-804D-9B6D-B84B64535EA1}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
+    <col min="4" max="4" width="11.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="24">
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>633515</v>
+      </c>
+      <c r="C8">
+        <v>4.2698340000000004</v>
+      </c>
+      <c r="D8">
+        <v>1.125985</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9">
+        <v>2622</v>
+      </c>
+      <c r="C9">
+        <v>4.0614039999999996</v>
+      </c>
+      <c r="D9">
+        <v>0.91640600000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3">
+        <f>C8</f>
+        <v>4.2698340000000004</v>
+      </c>
+      <c r="B12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3">
+        <f>C9</f>
+        <v>4.0614039999999996</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3">
+        <f>D8^2</f>
+        <v>1.2678422202249999</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3">
+        <f>D9^2</f>
+        <v>0.83979995683600006</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="4">
+        <f>B8</f>
+        <v>633515</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="4">
+        <f>B9</f>
+        <v>2622</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="3">
+        <f>SQRT(((A16-1)*A14+(A17-1)*A15)/(A16+A17-2))</f>
+        <v>1.125201583182917</v>
+      </c>
+      <c r="B18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="5">
+        <f>(A12-A13)/(A18*SQRT(1/A16+1/A17))</f>
+        <v>9.4656264293079211</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="5">
+        <f>(A14/A16+A15/A17)^2/((A14/A16)^2/(A16-1)+(A15/A17)^2/(A17-1))</f>
+        <v>2653.855735515669</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="2">
+        <v>0.95</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="12">
+        <f>TDIST(A19,A20,1)</f>
+        <v>3.1085850145084984E-21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="69" customHeight="1">
+      <c r="A24" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>